<commit_message>
correct bug triggering inputs
</commit_message>
<xml_diff>
--- a/bug triggering inputs/record.xlsx
+++ b/bug triggering inputs/record.xlsx
@@ -152,10 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Confirmed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://gcc.gnu.org/bugzilla/show_bug.cgi?id=113916</t>
   </si>
   <si>
@@ -187,6 +183,10 @@
   </si>
   <si>
     <t>Already Fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duplicate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -558,7 +558,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -659,16 +659,16 @@
         <v>32</v>
       </c>
       <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -725,44 +725,44 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>